<commit_message>
not much has changed, just some more analysis
</commit_message>
<xml_diff>
--- a/codebook_peter.xlsx
+++ b/codebook_peter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\coding projects\DS4Org\DS4ORG_unibe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7564A9D7-C9D5-42FD-987E-346CDECB6A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2C3E7F-131A-42D0-9BB1-85D7ED2E3A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="92">
   <si>
     <t>Are you self-employed?</t>
   </si>
@@ -300,6 +300,21 @@
   </si>
   <si>
     <t>all nan values are category 0</t>
+  </si>
+  <si>
+    <t>The value is only 1 if the previous column has value 0, so this is pretty unnecessary</t>
+  </si>
+  <si>
+    <t>Not eligible for coverage / N/A</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>I don't know</t>
   </si>
 </sst>
 </file>
@@ -662,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-  <dimension ref="A1:M126"/>
+  <dimension ref="A1:M124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,50 +811,65 @@
       <c r="B5" t="s">
         <v>65</v>
       </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
+    </row>
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -856,109 +886,82 @@
       <c r="H8">
         <v>4</v>
       </c>
-      <c r="I8">
+    </row>
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-      <c r="J10">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="B12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>66</v>
@@ -966,7 +969,7 @@
     </row>
     <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>65</v>
@@ -974,7 +977,7 @@
     </row>
     <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>66</v>
@@ -982,7 +985,7 @@
     </row>
     <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
@@ -990,71 +993,71 @@
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
@@ -1062,7 +1065,7 @@
     </row>
     <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
         <v>65</v>
@@ -1070,39 +1073,39 @@
     </row>
     <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>66</v>
@@ -1110,7 +1113,7 @@
     </row>
     <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
         <v>65</v>
@@ -1118,7 +1121,7 @@
     </row>
     <row r="38" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
@@ -1126,7 +1129,7 @@
     </row>
     <row r="39" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
         <v>65</v>
@@ -1134,7 +1137,7 @@
     </row>
     <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
         <v>66</v>
@@ -1142,7 +1145,7 @@
     </row>
     <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>65</v>
@@ -1150,103 +1153,103 @@
     </row>
     <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B48" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
         <v>66</v>
@@ -1254,7 +1257,7 @@
     </row>
     <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
         <v>65</v>
@@ -1262,39 +1265,39 @@
     </row>
     <row r="56" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
         <v>66</v>
@@ -1302,7 +1305,7 @@
     </row>
     <row r="61" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
         <v>65</v>
@@ -1310,23 +1313,23 @@
     </row>
     <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B63" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B64" t="s">
         <v>66</v>
@@ -1334,7 +1337,7 @@
     </row>
     <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B65" t="s">
         <v>65</v>
@@ -1342,7 +1345,7 @@
     </row>
     <row r="66" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B66" t="s">
         <v>66</v>
@@ -1350,7 +1353,7 @@
     </row>
     <row r="67" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
@@ -1358,23 +1361,23 @@
     </row>
     <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B70" t="s">
         <v>66</v>
@@ -1382,7 +1385,7 @@
     </row>
     <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B71" t="s">
         <v>65</v>
@@ -1390,55 +1393,55 @@
     </row>
     <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B72" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B75" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B76" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B77" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B78" t="s">
         <v>66</v>
@@ -1446,7 +1449,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B79" t="s">
         <v>65</v>
@@ -1454,87 +1457,87 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B80" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B83" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B85" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B86" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B87" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B88" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B89" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B90" t="s">
         <v>66</v>
@@ -1542,7 +1545,7 @@
     </row>
     <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B91" t="s">
         <v>65</v>
@@ -1550,7 +1553,7 @@
     </row>
     <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B92" t="s">
         <v>66</v>
@@ -1558,7 +1561,7 @@
     </row>
     <row r="93" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B93" t="s">
         <v>65</v>
@@ -1566,7 +1569,7 @@
     </row>
     <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B94" t="s">
         <v>66</v>
@@ -1574,7 +1577,7 @@
     </row>
     <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B95" t="s">
         <v>65</v>
@@ -1582,7 +1585,7 @@
     </row>
     <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B96" t="s">
         <v>66</v>
@@ -1590,7 +1593,7 @@
     </row>
     <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B97" t="s">
         <v>65</v>
@@ -1598,71 +1601,71 @@
     </row>
     <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B98" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B99" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B100" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B101" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B102" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B103" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B104" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B105" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B106" t="s">
         <v>66</v>
@@ -1670,7 +1673,7 @@
     </row>
     <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B107" t="s">
         <v>65</v>
@@ -1678,23 +1681,23 @@
     </row>
     <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B108" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B109" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B110" t="s">
         <v>66</v>
@@ -1702,7 +1705,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B111" t="s">
         <v>65</v>
@@ -1710,7 +1713,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B112" t="s">
         <v>66</v>
@@ -1718,7 +1721,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B113" t="s">
         <v>65</v>
@@ -1726,55 +1729,55 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B115" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B116" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B117" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B118" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B119" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B120" t="s">
         <v>66</v>
@@ -1782,7 +1785,7 @@
     </row>
     <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B121" t="s">
         <v>65</v>
@@ -1790,48 +1793,32 @@
     </row>
     <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B122" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B123" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B124" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B125" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B126" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B126" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B126">
-      <sortCondition ref="B1:B126"/>
+  <autoFilter ref="A1:B124" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B124">
+      <sortCondition ref="B1:B124"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Got stuck on the gender column
</commit_message>
<xml_diff>
--- a/codebook_peter.xlsx
+++ b/codebook_peter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\coding projects\DS4Org\DS4ORG_unibe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2C3E7F-131A-42D0-9BB1-85D7ED2E3A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFBBF29-34DB-4749-A2F4-8B956DCA2B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$114</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="151">
   <si>
     <t>Are you self-employed?</t>
   </si>
@@ -293,9 +293,6 @@
     <t>nan</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -315,6 +312,186 @@
   </si>
   <si>
     <t>I don't know</t>
+  </si>
+  <si>
+    <t>I am not sure</t>
+  </si>
+  <si>
+    <t>Very easy</t>
+  </si>
+  <si>
+    <t>Somewhat easy</t>
+  </si>
+  <si>
+    <t>Neither easy nor difficult</t>
+  </si>
+  <si>
+    <t>Very difficult</t>
+  </si>
+  <si>
+    <t>Somewhat difficult</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>Yes, I know several</t>
+  </si>
+  <si>
+    <t>I know some</t>
+  </si>
+  <si>
+    <t>No, I don't know any</t>
+  </si>
+  <si>
+    <t>Sometimes, if it comes up</t>
+  </si>
+  <si>
+    <t>No, because it doesn't matter</t>
+  </si>
+  <si>
+    <t>No, because it would impact me negatively</t>
+  </si>
+  <si>
+    <t>Not applicable to me</t>
+  </si>
+  <si>
+    <t>Yes, always</t>
+  </si>
+  <si>
+    <t>I'm not sure</t>
+  </si>
+  <si>
+    <t>Unsure</t>
+  </si>
+  <si>
+    <t>1-25%</t>
+  </si>
+  <si>
+    <t>26-50%</t>
+  </si>
+  <si>
+    <t>51-75%</t>
+  </si>
+  <si>
+    <t>76-100%</t>
+  </si>
+  <si>
+    <t>Yes, they all did</t>
+  </si>
+  <si>
+    <t>Some did</t>
+  </si>
+  <si>
+    <t>No, none did</t>
+  </si>
+  <si>
+    <t>Yes, I was aware of all of them</t>
+  </si>
+  <si>
+    <t>I was aware of some</t>
+  </si>
+  <si>
+    <t>No, I only became aware later</t>
+  </si>
+  <si>
+    <t>N/A (not currently aware)</t>
+  </si>
+  <si>
+    <t>None did</t>
+  </si>
+  <si>
+    <t>Sometimes</t>
+  </si>
+  <si>
+    <t>Some of them</t>
+  </si>
+  <si>
+    <t>Yes, all of them</t>
+  </si>
+  <si>
+    <t>None of them</t>
+  </si>
+  <si>
+    <t>Yes, at all of my previous employers</t>
+  </si>
+  <si>
+    <t>No, at none of my previous employers</t>
+  </si>
+  <si>
+    <t>Some of my previous employers</t>
+  </si>
+  <si>
+    <t>long text answers</t>
+  </si>
+  <si>
+    <t>No Nan answers</t>
+  </si>
+  <si>
+    <t>formatting issues, maybe delete this column? Or merge with previous column (index 39)</t>
+  </si>
+  <si>
+    <t>Yes, they do</t>
+  </si>
+  <si>
+    <t>Yes, I think they would</t>
+  </si>
+  <si>
+    <t>No, I don't think they would</t>
+  </si>
+  <si>
+    <t>No, they do not</t>
+  </si>
+  <si>
+    <t>Very open</t>
+  </si>
+  <si>
+    <t>Somewhat open</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Somewhat not open</t>
+  </si>
+  <si>
+    <t>Not open at all</t>
+  </si>
+  <si>
+    <t>Not applicable to me (I do not have a mental illness)</t>
+  </si>
+  <si>
+    <t>Yes, I experienced</t>
+  </si>
+  <si>
+    <t>Yes, I observed</t>
+  </si>
+  <si>
+    <t>Maybe/Not sure</t>
+  </si>
+  <si>
+    <t>multiple answers, could possibly also be categorized</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Often</t>
+  </si>
+  <si>
+    <t>Rarely</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>all real values</t>
+  </si>
+  <si>
+    <t>many text answers</t>
   </si>
 </sst>
 </file>
@@ -677,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-  <dimension ref="A1:M124"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +873,7 @@
         <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
         <v>67</v>
@@ -734,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -780,7 +957,7 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -829,7 +1006,7 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>83</v>
@@ -849,16 +1026,16 @@
         <v>83</v>
       </c>
       <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
         <v>89</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>90</v>
       </c>
-      <c r="G7" t="s">
-        <v>91</v>
-      </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -869,7 +1046,7 @@
         <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -894,6 +1071,18 @@
       <c r="B9" t="s">
         <v>65</v>
       </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -902,6 +1091,21 @@
       <c r="B10" t="s">
         <v>66</v>
       </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -910,6 +1114,18 @@
       <c r="B11" t="s">
         <v>65</v>
       </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -918,6 +1134,21 @@
       <c r="B12" t="s">
         <v>66</v>
       </c>
+      <c r="C12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -926,6 +1157,18 @@
       <c r="B13" t="s">
         <v>65</v>
       </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -934,6 +1177,21 @@
       <c r="B14" t="s">
         <v>66</v>
       </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -942,6 +1200,18 @@
       <c r="B15" t="s">
         <v>65</v>
       </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -950,770 +1220,1919 @@
       <c r="B16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B22" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B27" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" t="s">
+        <v>102</v>
+      </c>
+      <c r="I34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" t="s">
+        <v>110</v>
+      </c>
+      <c r="H44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B47" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" t="s">
+        <v>114</v>
+      </c>
+      <c r="H47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B48" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" t="s">
+        <v>117</v>
+      </c>
+      <c r="H49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="H50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B51" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" t="s">
+        <v>113</v>
+      </c>
+      <c r="G51" t="s">
+        <v>119</v>
+      </c>
+      <c r="H51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="H52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" t="s">
+        <v>112</v>
+      </c>
+      <c r="F53" t="s">
+        <v>113</v>
+      </c>
+      <c r="G53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" t="s">
+        <v>105</v>
+      </c>
+      <c r="F55" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" t="s">
+        <v>88</v>
+      </c>
+      <c r="H55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E57" t="s">
+        <v>122</v>
+      </c>
+      <c r="F57" t="s">
+        <v>121</v>
+      </c>
+      <c r="G57" t="s">
+        <v>123</v>
+      </c>
+      <c r="H57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B58" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B59" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" t="s">
+        <v>122</v>
+      </c>
+      <c r="F59" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B61" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>83</v>
+      </c>
+      <c r="E61" t="s">
+        <v>124</v>
+      </c>
+      <c r="F61" t="s">
+        <v>126</v>
+      </c>
+      <c r="G61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B62" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="G62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B63" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>83</v>
+      </c>
+      <c r="E63" t="s">
+        <v>124</v>
+      </c>
+      <c r="F63" t="s">
+        <v>126</v>
+      </c>
+      <c r="G63" t="s">
+        <v>125</v>
+      </c>
+      <c r="H63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B64" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <v>3</v>
+      </c>
+      <c r="H64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65" t="s">
+        <v>112</v>
+      </c>
+      <c r="F65" t="s">
+        <v>113</v>
+      </c>
+      <c r="G65" t="s">
+        <v>119</v>
+      </c>
+      <c r="H65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>85</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
+        <v>3</v>
+      </c>
+      <c r="H66">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>83</v>
+      </c>
+      <c r="E67" t="s">
+        <v>122</v>
+      </c>
+      <c r="F67" t="s">
+        <v>121</v>
+      </c>
+      <c r="G67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>2</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>88</v>
+      </c>
+      <c r="E69" t="s">
+        <v>89</v>
+      </c>
+      <c r="F69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>128</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D72" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" t="s">
+        <v>89</v>
+      </c>
+      <c r="F72" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B73" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C73" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B75" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D76" t="s">
+        <v>130</v>
+      </c>
+      <c r="E76" t="s">
+        <v>131</v>
+      </c>
+      <c r="F76" t="s">
+        <v>97</v>
+      </c>
+      <c r="G76" t="s">
+        <v>132</v>
+      </c>
+      <c r="H76" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C77" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <v>3</v>
+      </c>
+      <c r="G77">
+        <v>4</v>
+      </c>
+      <c r="H77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D78" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" t="s">
+        <v>135</v>
+      </c>
+      <c r="F78" t="s">
+        <v>136</v>
+      </c>
+      <c r="G78" t="s">
+        <v>137</v>
+      </c>
+      <c r="H78" t="s">
+        <v>138</v>
+      </c>
+      <c r="I78" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C79" t="s">
+        <v>128</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+      <c r="H79">
+        <v>5</v>
+      </c>
+      <c r="I79">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D80" t="s">
+        <v>83</v>
+      </c>
+      <c r="E80" t="s">
+        <v>140</v>
+      </c>
+      <c r="F80" t="s">
+        <v>141</v>
+      </c>
+      <c r="G80" t="s">
+        <v>142</v>
+      </c>
+      <c r="H80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C81" t="s">
+        <v>85</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="F81">
+        <v>2</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+      <c r="H81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D82" t="s">
+        <v>83</v>
+      </c>
+      <c r="E82" t="s">
+        <v>89</v>
+      </c>
+      <c r="F82" t="s">
+        <v>97</v>
+      </c>
+      <c r="G82" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B83" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C83" t="s">
+        <v>85</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D84" t="s">
+        <v>89</v>
+      </c>
+      <c r="E84" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B85" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C85" t="s">
+        <v>128</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>2</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B86" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D86" t="s">
+        <v>89</v>
+      </c>
+      <c r="E86" t="s">
+        <v>97</v>
+      </c>
+      <c r="F86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B87" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C87" t="s">
+        <v>128</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>2</v>
+      </c>
+      <c r="F87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B88" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D88" t="s">
+        <v>89</v>
+      </c>
+      <c r="E88" t="s">
+        <v>97</v>
+      </c>
+      <c r="F88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B89" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C89" t="s">
+        <v>128</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B90" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C90" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B91" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B92" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D92" t="s">
+        <v>89</v>
+      </c>
+      <c r="E92" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B93" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C93" t="s">
+        <v>128</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C94" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B95" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D96" t="s">
+        <v>145</v>
+      </c>
+      <c r="E96" t="s">
+        <v>120</v>
+      </c>
+      <c r="F96" t="s">
+        <v>146</v>
+      </c>
+      <c r="G96" t="s">
+        <v>147</v>
+      </c>
+      <c r="H96" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B97" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C97" t="s">
+        <v>128</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>2</v>
+      </c>
+      <c r="F97">
+        <v>3</v>
+      </c>
+      <c r="G97">
+        <v>4</v>
+      </c>
+      <c r="H97">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B98" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D98" t="s">
+        <v>145</v>
+      </c>
+      <c r="E98" t="s">
+        <v>120</v>
+      </c>
+      <c r="F98" t="s">
+        <v>146</v>
+      </c>
+      <c r="G98" t="s">
+        <v>147</v>
+      </c>
+      <c r="H98" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B99" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C99" t="s">
+        <v>128</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>2</v>
+      </c>
+      <c r="F99">
+        <v>3</v>
+      </c>
+      <c r="G99">
+        <v>4</v>
+      </c>
+      <c r="H99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="C100" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B101" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B102" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B103" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B105" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B106" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B107" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B108" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B109" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B110" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B111" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B112" t="s">
         <v>66</v>
@@ -1721,7 +3140,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B113" t="s">
         <v>65</v>
@@ -1729,96 +3148,16 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B114" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B115" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B116" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B117" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B118" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B119" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B120" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B121" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B122" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B123" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B124" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B124" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B124">
-      <sortCondition ref="B1:B124"/>
+  <autoFilter ref="A1:B114" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B114">
+      <sortCondition ref="B1:B114"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
mostly finished the categorization of the variables
</commit_message>
<xml_diff>
--- a/codebook_peter.xlsx
+++ b/codebook_peter.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\coding projects\DS4Org\DS4ORG_unibe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFBBF29-34DB-4749-A2F4-8B956DCA2B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF97282-76F8-4B4E-B19E-CA6EA6540720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$109</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="157">
   <si>
     <t>Are you self-employed?</t>
   </si>
@@ -492,6 +492,24 @@
   </si>
   <si>
     <t>many text answers</t>
+  </si>
+  <si>
+    <t>'female', 'Female', 'I identify as female.', 'female ', 'Female assigned at birth ', 'F', 'Woman', 'f', 'Cis female ', 'Female ', 'woman', 'female/woman', 'Female (props for making this a freeform field, though)', ' Female', 'Cis-woman', 'Cisgender Female'</t>
+  </si>
+  <si>
+    <t>Male', 'male', 'Male ', 'M', 'm', 'man', 'Cis male', 'Male.', 'Male (cis)', 'Sex is male', 'cis male', 'Dude', "I'm a man why didn't you make this a drop down question. You should of asked sex? And I would of answered yes please. Seriously how much text can this take? ", 'male ', 'Cis Male', 'cisdude', 'cis man', 'MALE', 'Man'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bigender', 'non-binary', 'fm', 'Transitioned, M2F', 'Genderfluid (born female)', 'Other/Transfeminine', 'Female or Multi-Gender Femme', 'Androgynous', 'male 9:1 female, roughly',  'Other', 'nb masculine', 'none of your business', 'genderqueer', 'Human', 'Genderfluid','Enby', 'Malr', 'genderqueer woman', 'mtf', 'Queer', 'Agender', 'Fluid', 'mail', 'M|', 'Male/genderqueer', 'fem', 'Nonbinary', 'human', 'Unicorn', 'Male (trans, FtM)', 'Genderqueer', 'Genderflux demi-girl', 'female-bodied; no feelings about gender', 'AFAB', 'Transgender woman' </t>
+  </si>
+  <si>
+    <t>all nan values are category 3</t>
+  </si>
+  <si>
+    <t>String Value is fine here</t>
+  </si>
+  <si>
+    <t>Always</t>
   </si>
 </sst>
 </file>
@@ -533,13 +551,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -854,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="F115" sqref="F114:F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,6 +3068,18 @@
       <c r="C101" t="s">
         <v>150</v>
       </c>
+      <c r="D101" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E101" t="s">
+        <v>151</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G101" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
@@ -3057,6 +3088,21 @@
       <c r="B102" t="s">
         <v>66</v>
       </c>
+      <c r="C102" t="s">
+        <v>154</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102">
+        <v>3</v>
+      </c>
+      <c r="G102">
+        <v>3</v>
+      </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
@@ -3065,99 +3111,92 @@
       <c r="B103" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C104" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B105" t="s">
         <v>65</v>
+      </c>
+      <c r="C105" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C106" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B107" t="s">
         <v>65</v>
+      </c>
+      <c r="C107" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B108" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D108" t="s">
+        <v>156</v>
+      </c>
+      <c r="E108" t="s">
+        <v>120</v>
+      </c>
+      <c r="F108" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B109" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B110" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B111" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B112" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B113" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B114" t="s">
-        <v>66</v>
+        <v>66</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>2</v>
+      </c>
+      <c r="F109">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B114" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B114">
-      <sortCondition ref="B1:B114"/>
+  <autoFilter ref="A1:B109" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B109">
+      <sortCondition ref="B1:B109"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
decided what should be added to the regression
</commit_message>
<xml_diff>
--- a/codebook_peter.xlsx
+++ b/codebook_peter.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\coding projects\DS4Org\DS4ORG_unibe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Desktop/Whatever/code/DS4Org/DS4ORG_unibe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF97282-76F8-4B4E-B19E-CA6EA6540720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A191B6DB-DBED-8A4B-AE7F-9FE450EA0909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
+    <workbookView xWindow="6880" yWindow="500" windowWidth="21920" windowHeight="17500" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$A$110</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="159">
   <si>
     <t>Are you self-employed?</t>
   </si>
@@ -510,6 +508,12 @@
   </si>
   <si>
     <t>Always</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>non-USA</t>
   </si>
 </sst>
 </file>
@@ -531,12 +535,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -551,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -559,6 +581,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -873,18 +907,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-  <dimension ref="A1:M109"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="F115" sqref="F114:F115"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -925,7 +964,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -939,8 +978,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -968,7 +1007,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1000,7 +1039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1034,8 +1073,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -1057,7 +1096,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1083,8 +1122,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
@@ -1103,7 +1142,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1126,8 +1165,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
@@ -1146,7 +1185,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1169,8 +1208,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
@@ -1189,7 +1228,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1212,8 +1251,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
@@ -1232,7 +1271,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1255,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1284,7 +1323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1316,8 +1355,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
@@ -1336,7 +1375,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1359,8 +1398,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
@@ -1379,7 +1418,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1402,8 +1441,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B23" t="s">
@@ -1422,7 +1461,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1445,8 +1484,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B25" t="s">
@@ -1465,7 +1504,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -1488,8 +1527,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B27" t="s">
@@ -1508,7 +1547,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -1531,8 +1570,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B29" t="s">
@@ -1548,7 +1587,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1568,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -1605,7 +1644,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -1628,7 +1667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1654,7 +1693,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -1683,8 +1722,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B36" t="s">
@@ -1703,7 +1742,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1726,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1752,7 +1791,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
@@ -1781,8 +1820,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B40" t="s">
@@ -1804,7 +1843,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -1830,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>22</v>
       </c>
@@ -1853,7 +1892,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
@@ -1879,8 +1918,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B44" t="s">
@@ -1902,7 +1941,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1928,7 +1967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -1942,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -1965,7 +2004,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -1991,7 +2030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2014,7 +2053,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -2040,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -2063,7 +2102,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>27</v>
       </c>
@@ -2089,7 +2128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>28</v>
       </c>
@@ -2109,7 +2148,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>28</v>
       </c>
@@ -2132,7 +2171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2155,7 +2194,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>29</v>
       </c>
@@ -2181,7 +2220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>30</v>
       </c>
@@ -2204,7 +2243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>30</v>
       </c>
@@ -2230,7 +2269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>31</v>
       </c>
@@ -2250,7 +2289,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>31</v>
       </c>
@@ -2273,7 +2312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>32</v>
       </c>
@@ -2293,7 +2332,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>32</v>
       </c>
@@ -2316,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
@@ -2339,7 +2378,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>33</v>
       </c>
@@ -2365,7 +2404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>34</v>
       </c>
@@ -2388,7 +2427,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>34</v>
       </c>
@@ -2414,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
@@ -2434,7 +2473,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
@@ -2457,7 +2496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>36</v>
       </c>
@@ -2474,7 +2513,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>36</v>
       </c>
@@ -2494,7 +2533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>37</v>
       </c>
@@ -2505,7 +2544,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>38</v>
       </c>
@@ -2522,7 +2561,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>38</v>
       </c>
@@ -2542,7 +2581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>39</v>
       </c>
@@ -2553,7 +2592,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>40</v>
       </c>
@@ -2564,8 +2603,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B76" t="s">
@@ -2587,7 +2626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>41</v>
       </c>
@@ -2613,7 +2652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>42</v>
       </c>
@@ -2639,7 +2678,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
@@ -2668,8 +2707,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B80" t="s">
@@ -2691,7 +2730,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
@@ -2717,7 +2756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>44</v>
       </c>
@@ -2737,7 +2776,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>44</v>
       </c>
@@ -2760,7 +2799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
@@ -2777,7 +2816,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>45</v>
       </c>
@@ -2797,8 +2836,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A86" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B86" t="s">
@@ -2814,7 +2853,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>46</v>
       </c>
@@ -2834,8 +2873,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B88" t="s">
@@ -2851,7 +2890,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>47</v>
       </c>
@@ -2871,7 +2910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>48</v>
       </c>
@@ -2882,7 +2921,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>49</v>
       </c>
@@ -2893,8 +2932,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A92" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B92" t="s">
@@ -2907,7 +2946,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>50</v>
       </c>
@@ -2924,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>51</v>
       </c>
@@ -2935,7 +2974,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>52</v>
       </c>
@@ -2949,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>53</v>
       </c>
@@ -2972,7 +3011,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>53</v>
       </c>
@@ -2998,7 +3037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>54</v>
       </c>
@@ -3021,7 +3060,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>54</v>
       </c>
@@ -3047,8 +3086,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B100" t="s">
@@ -3058,8 +3097,8 @@
         <v>149</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B101" t="s">
@@ -3081,7 +3120,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>56</v>
       </c>
@@ -3104,31 +3143,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B103" t="s">
         <v>65</v>
       </c>
-      <c r="C103" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="D103" t="s">
+        <v>157</v>
+      </c>
+      <c r="E103" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B104" t="s">
+        <v>66</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B104" t="s">
-        <v>65</v>
-      </c>
-      <c r="C104" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="B105" t="s">
         <v>65</v>
@@ -3137,9 +3182,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B106" t="s">
         <v>65</v>
@@ -3148,55 +3193,66 @@
         <v>155</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B107" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B107" t="s">
-        <v>65</v>
-      </c>
-      <c r="C107" t="s">
+      <c r="B108" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B108" t="s">
-        <v>65</v>
-      </c>
-      <c r="D108" t="s">
+      <c r="B109" t="s">
+        <v>65</v>
+      </c>
+      <c r="D109" t="s">
         <v>156</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E109" t="s">
         <v>120</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F109" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+    <row r="110" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B109" t="s">
-        <v>66</v>
-      </c>
-      <c r="D109">
-        <v>1</v>
-      </c>
-      <c r="E109">
-        <v>2</v>
-      </c>
-      <c r="F109">
+      <c r="B110" t="s">
+        <v>66</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>2</v>
+      </c>
+      <c r="F110">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B109" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B109">
-      <sortCondition ref="B1:B109"/>
+  <autoFilter ref="A1:B110" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B110">
+      <sortCondition ref="B1:B110"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
changed the order of some variables to make it more sense. created the first regressions
</commit_message>
<xml_diff>
--- a/codebook_peter.xlsx
+++ b/codebook_peter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peter/Desktop/Whatever/code/DS4Org/DS4ORG_unibe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\coding projects\DS4Org\DS4ORG_unibe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A191B6DB-DBED-8A4B-AE7F-9FE450EA0909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0CFF7F-6A4A-4BF7-B427-420C086D6063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="500" windowWidth="21920" windowHeight="17500" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
+    <workbookView xWindow="-16320" yWindow="-6870" windowWidth="16440" windowHeight="28320" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="162">
   <si>
     <t>Are you self-employed?</t>
   </si>
@@ -300,9 +300,6 @@
     <t>The value is only 1 if the previous column has value 0, so this is pretty unnecessary</t>
   </si>
   <si>
-    <t>Not eligible for coverage / N/A</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -514,6 +511,18 @@
   </si>
   <si>
     <t>non-USA</t>
+  </si>
+  <si>
+    <t>No, Not eligible for coverage / N/A</t>
+  </si>
+  <si>
+    <t>all nan values are category 2</t>
+  </si>
+  <si>
+    <t>all nan values are category 6</t>
+  </si>
+  <si>
+    <t>all nan values are category 4</t>
   </si>
 </sst>
 </file>
@@ -573,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -585,9 +594,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -909,21 +915,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="109" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -964,12 +970,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -978,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1007,7 +1013,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1056,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1073,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1090,13 +1096,10 @@
         <v>89</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1104,10 +1107,10 @@
         <v>66</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1118,11 +1121,8 @@
       <c r="G8">
         <v>3</v>
       </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1136,13 +1136,13 @@
         <v>88</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1150,10 +1150,10 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1165,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
@@ -1179,13 +1179,13 @@
         <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1193,10 +1193,10 @@
         <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1208,7 +1208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1225,10 +1225,10 @@
         <v>89</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1236,10 +1236,10 @@
         <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1251,7 +1251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -1268,10 +1268,10 @@
         <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1279,10 +1279,10 @@
         <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1305,25 +1305,25 @@
         <v>83</v>
       </c>
       <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
         <v>92</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>93</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" t="s">
         <v>94</v>
       </c>
-      <c r="H17" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" t="s">
-        <v>95</v>
-      </c>
       <c r="J17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
@@ -1369,13 +1369,13 @@
         <v>88</v>
       </c>
       <c r="F19" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1383,10 +1383,10 @@
         <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1398,8 +1398,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B21" t="s">
@@ -1412,13 +1412,13 @@
         <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1426,10 +1426,10 @@
         <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1441,7 +1441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -1455,13 +1455,13 @@
         <v>88</v>
       </c>
       <c r="F23" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1469,10 +1469,10 @@
         <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1484,7 +1484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>13</v>
       </c>
@@ -1498,13 +1498,13 @@
         <v>88</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -1512,10 +1512,10 @@
         <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1527,7 +1527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>14</v>
       </c>
@@ -1544,10 +1544,10 @@
         <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -1555,10 +1555,10 @@
         <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -1584,10 +1584,10 @@
         <v>88</v>
       </c>
       <c r="F29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1595,10 +1595,10 @@
         <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1607,12 +1607,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
         <v>83</v>
@@ -1624,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -1635,16 +1635,16 @@
         <v>83</v>
       </c>
       <c r="E32" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" t="s">
         <v>98</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>99</v>
       </c>
-      <c r="G32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1678,22 +1678,22 @@
         <v>83</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" t="s">
+        <v>102</v>
+      </c>
+      <c r="H34" t="s">
         <v>101</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" t="s">
         <v>103</v>
       </c>
-      <c r="H34" t="s">
-        <v>102</v>
-      </c>
-      <c r="I34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>19</v>
       </c>
@@ -1736,13 +1736,13 @@
         <v>88</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="G36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1750,10 +1750,10 @@
         <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1765,7 +1765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>20</v>
       </c>
@@ -1776,22 +1776,22 @@
         <v>83</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" t="s">
         <v>101</v>
       </c>
-      <c r="G38" t="s">
+      <c r="I38" t="s">
         <v>103</v>
       </c>
-      <c r="H38" t="s">
-        <v>102</v>
-      </c>
-      <c r="I38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>20</v>
       </c>
@@ -1799,10 +1799,10 @@
         <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>160</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1820,7 +1820,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>21</v>
       </c>
@@ -1834,16 +1834,16 @@
         <v>88</v>
       </c>
       <c r="F40" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="G40" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>21</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1869,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>22</v>
       </c>
@@ -1880,19 +1880,19 @@
         <v>83</v>
       </c>
       <c r="E42" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" t="s">
         <v>88</v>
       </c>
-      <c r="F42" t="s">
-        <v>89</v>
-      </c>
       <c r="G42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H42" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>22</v>
       </c>
@@ -1918,8 +1918,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B44" t="s">
@@ -1929,19 +1929,19 @@
         <v>83</v>
       </c>
       <c r="E44" t="s">
+        <v>107</v>
+      </c>
+      <c r="F44" t="s">
         <v>108</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>109</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>110</v>
       </c>
-      <c r="H44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -1967,12 +1967,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1981,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
@@ -1992,19 +1992,19 @@
         <v>83</v>
       </c>
       <c r="E47" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" t="s">
         <v>112</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>113</v>
       </c>
-      <c r="G47" t="s">
-        <v>114</v>
-      </c>
       <c r="H47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>25</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>26</v>
       </c>
@@ -2041,19 +2041,19 @@
         <v>83</v>
       </c>
       <c r="E49" t="s">
+        <v>114</v>
+      </c>
+      <c r="F49" t="s">
         <v>115</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>116</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>117</v>
       </c>
-      <c r="H49" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>26</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>27</v>
       </c>
@@ -2090,19 +2090,19 @@
         <v>83</v>
       </c>
       <c r="E51" t="s">
+        <v>111</v>
+      </c>
+      <c r="F51" t="s">
         <v>112</v>
       </c>
-      <c r="F51" t="s">
-        <v>113</v>
-      </c>
       <c r="G51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H51" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>27</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>28</v>
       </c>
@@ -2139,16 +2139,16 @@
         <v>83</v>
       </c>
       <c r="E53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" t="s">
         <v>112</v>
       </c>
-      <c r="F53" t="s">
-        <v>113</v>
-      </c>
       <c r="G53" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>28</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2182,19 +2182,19 @@
         <v>83</v>
       </c>
       <c r="E55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>29</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>30</v>
       </c>
@@ -2231,19 +2231,19 @@
         <v>83</v>
       </c>
       <c r="E57" t="s">
+        <v>121</v>
+      </c>
+      <c r="F57" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" t="s">
         <v>122</v>
       </c>
-      <c r="F57" t="s">
-        <v>121</v>
-      </c>
-      <c r="G57" t="s">
-        <v>123</v>
-      </c>
       <c r="H57" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>30</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>31</v>
       </c>
@@ -2280,16 +2280,16 @@
         <v>83</v>
       </c>
       <c r="E59" t="s">
+        <v>121</v>
+      </c>
+      <c r="F59" t="s">
+        <v>120</v>
+      </c>
+      <c r="G59" t="s">
         <v>122</v>
       </c>
-      <c r="F59" t="s">
-        <v>121</v>
-      </c>
-      <c r="G59" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>31</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>32</v>
       </c>
@@ -2323,16 +2323,16 @@
         <v>83</v>
       </c>
       <c r="E61" t="s">
+        <v>123</v>
+      </c>
+      <c r="F61" t="s">
+        <v>125</v>
+      </c>
+      <c r="G61" t="s">
         <v>124</v>
       </c>
-      <c r="F61" t="s">
-        <v>126</v>
-      </c>
-      <c r="G61" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>32</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
@@ -2366,19 +2366,19 @@
         <v>83</v>
       </c>
       <c r="E63" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" t="s">
+        <v>125</v>
+      </c>
+      <c r="G63" t="s">
         <v>124</v>
       </c>
-      <c r="F63" t="s">
-        <v>126</v>
-      </c>
-      <c r="G63" t="s">
-        <v>125</v>
-      </c>
       <c r="H63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>33</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>34</v>
       </c>
@@ -2415,19 +2415,19 @@
         <v>83</v>
       </c>
       <c r="E65" t="s">
+        <v>111</v>
+      </c>
+      <c r="F65" t="s">
         <v>112</v>
       </c>
-      <c r="F65" t="s">
-        <v>113</v>
-      </c>
       <c r="G65" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>34</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>35</v>
       </c>
@@ -2464,16 +2464,16 @@
         <v>83</v>
       </c>
       <c r="E67" t="s">
+        <v>121</v>
+      </c>
+      <c r="F67" t="s">
+        <v>120</v>
+      </c>
+      <c r="G67" t="s">
         <v>122</v>
       </c>
-      <c r="F67" t="s">
-        <v>121</v>
-      </c>
-      <c r="G67" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>35</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>36</v>
       </c>
@@ -2507,13 +2507,13 @@
         <v>88</v>
       </c>
       <c r="E69" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F69" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>36</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>66</v>
       </c>
       <c r="C70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2533,7 +2533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>37</v>
       </c>
@@ -2541,10 +2541,10 @@
         <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>38</v>
       </c>
@@ -2555,13 +2555,13 @@
         <v>88</v>
       </c>
       <c r="E72" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="F72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>38</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>66</v>
       </c>
       <c r="C73" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2581,7 +2581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>39</v>
       </c>
@@ -2589,10 +2589,10 @@
         <v>65</v>
       </c>
       <c r="C74" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>40</v>
       </c>
@@ -2600,10 +2600,10 @@
         <v>65</v>
       </c>
       <c r="C75" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>41</v>
       </c>
@@ -2611,22 +2611,22 @@
         <v>65</v>
       </c>
       <c r="D76" t="s">
+        <v>129</v>
+      </c>
+      <c r="E76" t="s">
         <v>130</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
+        <v>96</v>
+      </c>
+      <c r="G76" t="s">
         <v>131</v>
       </c>
-      <c r="F76" t="s">
-        <v>97</v>
-      </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>132</v>
       </c>
-      <c r="H76" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>41</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2652,7 +2652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>42</v>
       </c>
@@ -2660,25 +2660,25 @@
         <v>65</v>
       </c>
       <c r="D78" t="s">
+        <v>133</v>
+      </c>
+      <c r="E78" t="s">
         <v>134</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>135</v>
       </c>
-      <c r="F78" t="s">
+      <c r="G78" t="s">
         <v>136</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>137</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>138</v>
       </c>
-      <c r="I78" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>66</v>
       </c>
       <c r="C79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -2707,7 +2707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>43</v>
       </c>
@@ -2718,19 +2718,19 @@
         <v>83</v>
       </c>
       <c r="E80" t="s">
+        <v>139</v>
+      </c>
+      <c r="F80" t="s">
         <v>140</v>
       </c>
-      <c r="F80" t="s">
+      <c r="G80" t="s">
         <v>141</v>
       </c>
-      <c r="G80" t="s">
-        <v>142</v>
-      </c>
       <c r="H80" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>43</v>
       </c>
@@ -2738,10 +2738,10 @@
         <v>66</v>
       </c>
       <c r="C81" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2756,7 +2756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>44</v>
       </c>
@@ -2767,16 +2767,16 @@
         <v>83</v>
       </c>
       <c r="E82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F82" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G82" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>44</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>45</v>
       </c>
@@ -2807,16 +2807,16 @@
         <v>65</v>
       </c>
       <c r="D84" t="s">
+        <v>88</v>
+      </c>
+      <c r="E84" t="s">
+        <v>87</v>
+      </c>
+      <c r="F84" t="s">
         <v>89</v>
       </c>
-      <c r="E84" t="s">
-        <v>88</v>
-      </c>
-      <c r="F84" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>45</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>66</v>
       </c>
       <c r="C85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -2836,7 +2836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>46</v>
       </c>
@@ -2844,16 +2844,16 @@
         <v>65</v>
       </c>
       <c r="D86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F86" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>46</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>66</v>
       </c>
       <c r="C87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -2873,7 +2873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>47</v>
       </c>
@@ -2881,16 +2881,16 @@
         <v>65</v>
       </c>
       <c r="D88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E88" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F88" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>47</v>
       </c>
@@ -2898,7 +2898,7 @@
         <v>66</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D89">
         <v>1</v>
@@ -2910,7 +2910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>48</v>
       </c>
@@ -2918,10 +2918,10 @@
         <v>65</v>
       </c>
       <c r="C90" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>49</v>
       </c>
@@ -2929,10 +2929,10 @@
         <v>65</v>
       </c>
       <c r="C91" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>50</v>
       </c>
@@ -2940,13 +2940,13 @@
         <v>65</v>
       </c>
       <c r="D92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E92" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>50</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>66</v>
       </c>
       <c r="C93" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D93">
         <v>1</v>
@@ -2963,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>51</v>
       </c>
@@ -2971,15 +2971,15 @@
         <v>65</v>
       </c>
       <c r="C94" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B95" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2988,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>53</v>
       </c>
@@ -2996,22 +2996,22 @@
         <v>65</v>
       </c>
       <c r="D96" t="s">
+        <v>144</v>
+      </c>
+      <c r="E96" t="s">
+        <v>119</v>
+      </c>
+      <c r="F96" t="s">
         <v>145</v>
       </c>
-      <c r="E96" t="s">
-        <v>120</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>146</v>
       </c>
-      <c r="G96" t="s">
-        <v>147</v>
-      </c>
       <c r="H96" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>53</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>66</v>
       </c>
       <c r="C97" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -3037,7 +3037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>54</v>
       </c>
@@ -3045,22 +3045,22 @@
         <v>65</v>
       </c>
       <c r="D98" t="s">
+        <v>144</v>
+      </c>
+      <c r="E98" t="s">
+        <v>119</v>
+      </c>
+      <c r="F98" t="s">
         <v>145</v>
       </c>
-      <c r="E98" t="s">
-        <v>120</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="G98" t="s">
         <v>146</v>
       </c>
-      <c r="G98" t="s">
-        <v>147</v>
-      </c>
       <c r="H98" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>54</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>66</v>
       </c>
       <c r="C99" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -3086,18 +3086,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B100" t="s">
+        <v>147</v>
+      </c>
+      <c r="C100" t="s">
         <v>148</v>
       </c>
-      <c r="C100" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>56</v>
       </c>
@@ -3105,22 +3105,22 @@
         <v>65</v>
       </c>
       <c r="C101" t="s">
+        <v>149</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E101" t="s">
         <v>150</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="F101" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E101" t="s">
-        <v>151</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="G101" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>56</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>66</v>
       </c>
       <c r="C102" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D102">
         <v>1</v>
@@ -3143,7 +3143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>57</v>
       </c>
@@ -3151,14 +3151,14 @@
         <v>65</v>
       </c>
       <c r="D103" t="s">
+        <v>156</v>
+      </c>
+      <c r="E103" t="s">
         <v>157</v>
       </c>
-      <c r="E103" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="7" t="s">
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B104" t="s">
@@ -3171,7 +3171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>58</v>
       </c>
@@ -3179,10 +3179,10 @@
         <v>65</v>
       </c>
       <c r="C105" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>59</v>
       </c>
@@ -3190,10 +3190,10 @@
         <v>65</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>60</v>
       </c>
@@ -3201,10 +3201,10 @@
         <v>65</v>
       </c>
       <c r="C107" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>61</v>
       </c>
@@ -3212,10 +3212,10 @@
         <v>65</v>
       </c>
       <c r="C108" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>62</v>
       </c>
@@ -3223,16 +3223,16 @@
         <v>65</v>
       </c>
       <c r="D109" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F109" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
started clustering. K-means with 3 clusters is not looking good
</commit_message>
<xml_diff>
--- a/codebook_peter.xlsx
+++ b/codebook_peter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\coding projects\DS4Org\DS4ORG_unibe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0CFF7F-6A4A-4BF7-B427-420C086D6063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA51E71F-8835-4BF4-9F6C-DF8F1F1B2E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6870" windowWidth="16440" windowHeight="28320" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5A21C25D-713D-4B98-B5A1-A257BFB316EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,12 +560,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -915,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B748F300-CE8A-4BE0-BE39-31DF20A81F7E}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="109" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="109" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1602,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B31" t="s">
@@ -1723,7 +1717,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B36" t="s">
@@ -1743,17 +1737,17 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1766,7 +1760,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B38" t="s">
@@ -1792,7 +1786,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B39" t="s">
@@ -1821,7 +1815,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B40" t="s">
@@ -1844,17 +1838,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B41" t="s">
         <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1870,7 +1864,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B42" t="s">
@@ -1893,7 +1887,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B43" t="s">

</xml_diff>